<commit_message>
agregacion consulta con cursores para poder traer los store procedures
</commit_message>
<xml_diff>
--- a/reporte.xlsx
+++ b/reporte.xlsx
@@ -477,6 +477,15 @@
           <t>Ingeniería de Sistemas</t>
         </is>
       </c>
+      <c r="E2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -36862,6 +36871,15 @@
         <is>
           <t>Ingeniería de Sistemas</t>
         </is>
+      </c>
+      <c r="E1823" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1823" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1823" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="1824">

</xml_diff>

<commit_message>
agregacion proteccion de rutas sin base modelo de acceso
</commit_message>
<xml_diff>
--- a/reporte.xlsx
+++ b/reporte.xlsx
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G2" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
@@ -8460,6 +8460,15 @@
           <t>Ingeniería de Sistemas</t>
         </is>
       </c>
+      <c r="E401" t="n">
+        <v>5</v>
+      </c>
+      <c r="F401" t="n">
+        <v>8</v>
+      </c>
+      <c r="G401" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="402">
       <c r="A402" t="n">
@@ -36873,13 +36882,13 @@
         </is>
       </c>
       <c r="E1823" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F1823" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G1823" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="1824">
@@ -44854,6 +44863,15 @@
         <is>
           <t>Ingeniería de Sistemas</t>
         </is>
+      </c>
+      <c r="E2222" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2222" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2222" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="2223">

</xml_diff>